<commit_message>
topo for andy (again)
</commit_message>
<xml_diff>
--- a/Topography/LaJara_TopoSurvey/LongProfile_Slope.xlsx
+++ b/Topography/LaJara_TopoSurvey/LongProfile_Slope.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\La_Jara\Topography\LaJara_TopoSurvey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2D31DC-9855-404E-A529-B85B8132D5C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7DCB0F-DFA0-4CDB-A3AE-E97F7C1889DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AB3008BA-383C-43BA-9CB8-F95DC604E1C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Full reach slope" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Downstream</t>
   </si>
@@ -57,6 +54,54 @@
   </si>
   <si>
     <t>Up S</t>
+  </si>
+  <si>
+    <t>Equipment</t>
+  </si>
+  <si>
+    <t>GW 1 XS</t>
+  </si>
+  <si>
+    <t>GW 2 XS</t>
+  </si>
+  <si>
+    <t>GW3 XS</t>
+  </si>
+  <si>
+    <t>Piezometer 1</t>
+  </si>
+  <si>
+    <t>Piezometer 2</t>
+  </si>
+  <si>
+    <t>GW4</t>
+  </si>
+  <si>
+    <t>Piezometer 3</t>
+  </si>
+  <si>
+    <t>GW5 XS</t>
+  </si>
+  <si>
+    <t>GW7 XS</t>
+  </si>
+  <si>
+    <t>GW6 XS</t>
+  </si>
+  <si>
+    <t>Piezometer 5</t>
+  </si>
+  <si>
+    <t>GW 8 XS</t>
+  </si>
+  <si>
+    <t>GW 9 XS</t>
+  </si>
+  <si>
+    <t>Piezometer 6</t>
+  </si>
+  <si>
+    <t>Piezometer 4</t>
   </si>
 </sst>
 </file>
@@ -100,10 +145,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1051,7 +1096,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Full reach slope'!$D$3:$D$97</c:f>
+              <c:f>'Full reach slope'!$E$3:$E$97</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="95"/>
@@ -1345,7 +1390,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Full reach slope'!$E$3:$E$97</c:f>
+              <c:f>'Full reach slope'!$F$3:$F$97</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="95"/>
@@ -2947,13 +2992,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>525780</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>220980</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -2985,13 +3030,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>335280</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>30480</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
@@ -3022,1217 +3067,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="TP1 (3&amp;25)"/>
-      <sheetName val="TP2 (8)"/>
-      <sheetName val="TP3 (2)"/>
-      <sheetName val="TP5 (4)"/>
-      <sheetName val="TP6 (5)"/>
-      <sheetName val="TP7 (6)"/>
-      <sheetName val="TP8 (7)"/>
-      <sheetName val="Downstream"/>
-      <sheetName val="Upstream"/>
-      <sheetName val="RMSE"/>
-      <sheetName val="Full reach slope"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10">
-        <row r="3">
-          <cell r="D3">
-            <v>0</v>
-          </cell>
-          <cell r="E3">
-            <v>2732.8400000000011</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="D4">
-            <v>0.70000000000000284</v>
-          </cell>
-          <cell r="E4">
-            <v>2733.0300000000007</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5">
-            <v>1</v>
-          </cell>
-          <cell r="E5">
-            <v>2732.9900000000007</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="D6">
-            <v>2</v>
-          </cell>
-          <cell r="E6">
-            <v>2732.9450000000011</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="D7">
-            <v>3</v>
-          </cell>
-          <cell r="E7">
-            <v>2733.0400000000009</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8">
-            <v>4</v>
-          </cell>
-          <cell r="E8">
-            <v>2733.0900000000011</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="D9">
-            <v>5</v>
-          </cell>
-          <cell r="E9">
-            <v>2733.1450000000009</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="D10">
-            <v>6</v>
-          </cell>
-          <cell r="E10">
-            <v>2733.2100000000009</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="D11">
-            <v>7</v>
-          </cell>
-          <cell r="E11">
-            <v>2733.2400000000007</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="D12">
-            <v>8</v>
-          </cell>
-          <cell r="E12">
-            <v>2733.295000000001</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="D13">
-            <v>9</v>
-          </cell>
-          <cell r="E13">
-            <v>2733.3300000000008</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="D14">
-            <v>9.6000000000000014</v>
-          </cell>
-          <cell r="E14">
-            <v>2733.3450000000007</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="D15">
-            <v>9.7999999999999972</v>
-          </cell>
-          <cell r="E15">
-            <v>2733.5850000000009</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="D16">
-            <v>10</v>
-          </cell>
-          <cell r="E16">
-            <v>2733.5700000000011</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="D17">
-            <v>11</v>
-          </cell>
-          <cell r="E17">
-            <v>2733.5950000000007</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="D18">
-            <v>11.600000000000001</v>
-          </cell>
-          <cell r="E18">
-            <v>2733.565000000001</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="D19">
-            <v>12</v>
-          </cell>
-          <cell r="E19">
-            <v>2733.7250000000008</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="D20">
-            <v>13.200000000000003</v>
-          </cell>
-          <cell r="E20">
-            <v>2733.6150000000007</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="D21">
-            <v>13.5</v>
-          </cell>
-          <cell r="E21">
-            <v>2733.7400000000007</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="D22">
-            <v>13.600000000000001</v>
-          </cell>
-          <cell r="E22">
-            <v>2733.880000000001</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="D23">
-            <v>14</v>
-          </cell>
-          <cell r="E23">
-            <v>2733.8750000000009</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="D24">
-            <v>14.600000000000001</v>
-          </cell>
-          <cell r="E24">
-            <v>2733.8300000000008</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="D25">
-            <v>15.299999999999997</v>
-          </cell>
-          <cell r="E25">
-            <v>2733.7650000000008</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="D26">
-            <v>15.700000000000003</v>
-          </cell>
-          <cell r="E26">
-            <v>2733.8700000000008</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="A27">
-            <v>11.799999999999997</v>
-          </cell>
-          <cell r="B27">
-            <v>2722.4319999999998</v>
-          </cell>
-          <cell r="D27">
-            <v>16</v>
-          </cell>
-          <cell r="E27">
-            <v>2734.0350000000008</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28">
-            <v>12.5</v>
-          </cell>
-          <cell r="B28">
-            <v>2722.4919999999997</v>
-          </cell>
-          <cell r="D28">
-            <v>17</v>
-          </cell>
-          <cell r="E28">
-            <v>2734.0400000000009</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29">
-            <v>13</v>
-          </cell>
-          <cell r="B29">
-            <v>2722.4719999999998</v>
-          </cell>
-          <cell r="D29">
-            <v>17.600000000000001</v>
-          </cell>
-          <cell r="E29">
-            <v>2734.0350000000008</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="A30">
-            <v>13.5</v>
-          </cell>
-          <cell r="B30">
-            <v>2722.4869999999996</v>
-          </cell>
-          <cell r="D30">
-            <v>18</v>
-          </cell>
-          <cell r="E30">
-            <v>2734.1800000000007</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="A31">
-            <v>14</v>
-          </cell>
-          <cell r="B31">
-            <v>2722.5719999999997</v>
-          </cell>
-          <cell r="D31">
-            <v>18.5</v>
-          </cell>
-          <cell r="E31">
-            <v>2734.1150000000007</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="A32">
-            <v>14.5</v>
-          </cell>
-          <cell r="B32">
-            <v>2722.6169999999997</v>
-          </cell>
-          <cell r="D32">
-            <v>19</v>
-          </cell>
-          <cell r="E32">
-            <v>2734.1650000000009</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="A33">
-            <v>15</v>
-          </cell>
-          <cell r="B33">
-            <v>2722.587</v>
-          </cell>
-          <cell r="D33">
-            <v>20</v>
-          </cell>
-          <cell r="E33">
-            <v>2734.2850000000008</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="A34">
-            <v>15.5</v>
-          </cell>
-          <cell r="B34">
-            <v>2722.587</v>
-          </cell>
-          <cell r="D34">
-            <v>20.5</v>
-          </cell>
-          <cell r="E34">
-            <v>2734.3200000000006</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="A35">
-            <v>16</v>
-          </cell>
-          <cell r="B35">
-            <v>2722.5519999999997</v>
-          </cell>
-          <cell r="D35">
-            <v>21</v>
-          </cell>
-          <cell r="E35">
-            <v>2734.3450000000007</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="A36">
-            <v>16.5</v>
-          </cell>
-          <cell r="B36">
-            <v>2722.5789999999997</v>
-          </cell>
-          <cell r="D36">
-            <v>22</v>
-          </cell>
-          <cell r="E36">
-            <v>2734.380000000001</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="A37">
-            <v>17</v>
-          </cell>
-          <cell r="B37">
-            <v>2722.5619999999999</v>
-          </cell>
-          <cell r="D37">
-            <v>23</v>
-          </cell>
-          <cell r="E37">
-            <v>2734.4300000000007</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="A38">
-            <v>17.5</v>
-          </cell>
-          <cell r="B38">
-            <v>2722.6519999999996</v>
-          </cell>
-          <cell r="D38">
-            <v>23.299999999999997</v>
-          </cell>
-          <cell r="E38">
-            <v>2734.3950000000009</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="A39">
-            <v>18.299999999999997</v>
-          </cell>
-          <cell r="B39">
-            <v>2722.6539999999995</v>
-          </cell>
-          <cell r="D39">
-            <v>23.6</v>
-          </cell>
-          <cell r="E39">
-            <v>2734.545000000001</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="A40">
-            <v>18.600000000000001</v>
-          </cell>
-          <cell r="B40">
-            <v>2722.7789999999995</v>
-          </cell>
-          <cell r="D40">
-            <v>24.6</v>
-          </cell>
-          <cell r="E40">
-            <v>2734.8450000000007</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="A41">
-            <v>19.100000000000001</v>
-          </cell>
-          <cell r="B41">
-            <v>2722.6989999999996</v>
-          </cell>
-          <cell r="D41">
-            <v>25</v>
-          </cell>
-          <cell r="E41">
-            <v>2734.5750000000007</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="A42">
-            <v>19.299999999999997</v>
-          </cell>
-          <cell r="B42">
-            <v>2723.0039999999995</v>
-          </cell>
-          <cell r="D42">
-            <v>25.299999999999997</v>
-          </cell>
-          <cell r="E42">
-            <v>2734.5600000000009</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="A43">
-            <v>19.5</v>
-          </cell>
-          <cell r="B43">
-            <v>2723.0239999999994</v>
-          </cell>
-          <cell r="D43">
-            <v>26</v>
-          </cell>
-          <cell r="E43">
-            <v>2735.0100000000007</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="A44">
-            <v>20</v>
-          </cell>
-          <cell r="B44">
-            <v>2723.0789999999997</v>
-          </cell>
-          <cell r="D44">
-            <v>26.700000000000003</v>
-          </cell>
-          <cell r="E44">
-            <v>2735.0800000000008</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="A45">
-            <v>20.5</v>
-          </cell>
-          <cell r="B45">
-            <v>2723.0739999999996</v>
-          </cell>
-          <cell r="D45">
-            <v>27</v>
-          </cell>
-          <cell r="E45">
-            <v>2735.025000000001</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="A46">
-            <v>20.700000000000003</v>
-          </cell>
-          <cell r="B46">
-            <v>2723.0039999999995</v>
-          </cell>
-          <cell r="D46">
-            <v>27.1</v>
-          </cell>
-          <cell r="E46">
-            <v>2735.0000000000009</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="A47">
-            <v>20.700000000000003</v>
-          </cell>
-          <cell r="B47">
-            <v>2723.0989999999997</v>
-          </cell>
-          <cell r="D47">
-            <v>27.6</v>
-          </cell>
-          <cell r="E47">
-            <v>2735.2300000000009</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="A48">
-            <v>21.4</v>
-          </cell>
-          <cell r="B48">
-            <v>2723.0489999999995</v>
-          </cell>
-          <cell r="D48">
-            <v>28</v>
-          </cell>
-          <cell r="E48">
-            <v>2735.1450000000009</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="A49">
-            <v>21.6</v>
-          </cell>
-          <cell r="B49">
-            <v>2723.1789999999996</v>
-          </cell>
-          <cell r="D49">
-            <v>29</v>
-          </cell>
-          <cell r="E49">
-            <v>2735.1600000000008</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="A50">
-            <v>22.715000000000003</v>
-          </cell>
-          <cell r="B50">
-            <v>2723.1889999999994</v>
-          </cell>
-          <cell r="D50">
-            <v>29.200000000000003</v>
-          </cell>
-          <cell r="E50">
-            <v>2735.3650000000007</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="A51">
-            <v>23</v>
-          </cell>
-          <cell r="B51">
-            <v>2723.1889999999994</v>
-          </cell>
-          <cell r="D51">
-            <v>29.700000000000003</v>
-          </cell>
-          <cell r="E51">
-            <v>2735.2700000000009</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="A52">
-            <v>23</v>
-          </cell>
-          <cell r="B52">
-            <v>2723.1689999999994</v>
-          </cell>
-          <cell r="D52">
-            <v>30</v>
-          </cell>
-          <cell r="E52">
-            <v>2735.2150000000006</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="A53">
-            <v>23.5</v>
-          </cell>
-          <cell r="B53">
-            <v>2723.1589999999997</v>
-          </cell>
-          <cell r="D53">
-            <v>30.5</v>
-          </cell>
-          <cell r="E53">
-            <v>2735.4600000000009</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="A54">
-            <v>24</v>
-          </cell>
-          <cell r="B54">
-            <v>2723.1489999999994</v>
-          </cell>
-          <cell r="D54">
-            <v>31</v>
-          </cell>
-          <cell r="E54">
-            <v>2735.4150000000009</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="A55">
-            <v>24.5</v>
-          </cell>
-          <cell r="B55">
-            <v>2723.1589999999997</v>
-          </cell>
-          <cell r="D55">
-            <v>32</v>
-          </cell>
-          <cell r="E55">
-            <v>2735.4600000000009</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="A56">
-            <v>25</v>
-          </cell>
-          <cell r="B56">
-            <v>2723.2389999999996</v>
-          </cell>
-          <cell r="D56">
-            <v>33</v>
-          </cell>
-          <cell r="E56">
-            <v>2735.4700000000007</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="A57">
-            <v>25.5</v>
-          </cell>
-          <cell r="B57">
-            <v>2723.2589999999996</v>
-          </cell>
-          <cell r="D57">
-            <v>33.5</v>
-          </cell>
-          <cell r="E57">
-            <v>2735.4800000000009</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="A58">
-            <v>25.9</v>
-          </cell>
-          <cell r="B58">
-            <v>2723.5189999999993</v>
-          </cell>
-          <cell r="D58">
-            <v>34.5</v>
-          </cell>
-          <cell r="E58">
-            <v>2736.1250000000009</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="A59">
-            <v>26.5</v>
-          </cell>
-          <cell r="B59">
-            <v>2723.4289999999996</v>
-          </cell>
-          <cell r="D59">
-            <v>35</v>
-          </cell>
-          <cell r="E59">
-            <v>2736.1150000000007</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="A60">
-            <v>26.9</v>
-          </cell>
-          <cell r="B60">
-            <v>2723.4489999999996</v>
-          </cell>
-          <cell r="D60">
-            <v>36</v>
-          </cell>
-          <cell r="E60">
-            <v>2736.0900000000006</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="A61">
-            <v>26.9</v>
-          </cell>
-          <cell r="B61">
-            <v>2723.4069999999997</v>
-          </cell>
-          <cell r="D61">
-            <v>36.299999999999997</v>
-          </cell>
-          <cell r="E61">
-            <v>2736.0350000000008</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="A62">
-            <v>27.5</v>
-          </cell>
-          <cell r="B62">
-            <v>2723.5189999999993</v>
-          </cell>
-          <cell r="D62">
-            <v>37</v>
-          </cell>
-          <cell r="E62">
-            <v>2736.420000000001</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="A63">
-            <v>27.799999999999997</v>
-          </cell>
-          <cell r="B63">
-            <v>2723.6589999999997</v>
-          </cell>
-          <cell r="D63">
-            <v>37.599999999999994</v>
-          </cell>
-          <cell r="E63">
-            <v>2736.440000000001</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="A64">
-            <v>28</v>
-          </cell>
-          <cell r="B64">
-            <v>2723.5789999999997</v>
-          </cell>
-          <cell r="D64">
-            <v>38</v>
-          </cell>
-          <cell r="E64">
-            <v>2736.4300000000007</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="A65">
-            <v>28.5</v>
-          </cell>
-          <cell r="B65">
-            <v>2723.7089999999994</v>
-          </cell>
-          <cell r="D65">
-            <v>39</v>
-          </cell>
-          <cell r="E65">
-            <v>2736.565000000001</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="A66">
-            <v>29</v>
-          </cell>
-          <cell r="B66">
-            <v>2723.6689999999994</v>
-          </cell>
-          <cell r="D66">
-            <v>40</v>
-          </cell>
-          <cell r="E66">
-            <v>2736.5150000000008</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="A67">
-            <v>29.5</v>
-          </cell>
-          <cell r="B67">
-            <v>2723.7089999999994</v>
-          </cell>
-          <cell r="D67">
-            <v>40.299999999999997</v>
-          </cell>
-          <cell r="E67">
-            <v>2736.7050000000008</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="A68">
-            <v>30</v>
-          </cell>
-          <cell r="B68">
-            <v>2723.8189999999995</v>
-          </cell>
-          <cell r="D68">
-            <v>41</v>
-          </cell>
-          <cell r="E68">
-            <v>2736.6450000000009</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="A69">
-            <v>30.5</v>
-          </cell>
-          <cell r="B69">
-            <v>2723.8389999999995</v>
-          </cell>
-          <cell r="D69">
-            <v>41.7</v>
-          </cell>
-          <cell r="E69">
-            <v>2736.610000000001</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="A70">
-            <v>31</v>
-          </cell>
-          <cell r="B70">
-            <v>2723.8389999999995</v>
-          </cell>
-          <cell r="D70">
-            <v>42</v>
-          </cell>
-          <cell r="E70">
-            <v>2736.7650000000008</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="A71">
-            <v>31.5</v>
-          </cell>
-          <cell r="B71">
-            <v>2723.8789999999995</v>
-          </cell>
-          <cell r="D71">
-            <v>42.599999999999994</v>
-          </cell>
-          <cell r="E71">
-            <v>2736.7890000000007</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="A72">
-            <v>32</v>
-          </cell>
-          <cell r="B72">
-            <v>2723.9239999999995</v>
-          </cell>
-          <cell r="D72">
-            <v>43</v>
-          </cell>
-          <cell r="E72">
-            <v>2736.8000000000011</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="A73">
-            <v>32.5</v>
-          </cell>
-          <cell r="B73">
-            <v>2723.8839999999996</v>
-          </cell>
-          <cell r="D73">
-            <v>43.5</v>
-          </cell>
-          <cell r="E73">
-            <v>2736.735000000001</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="A74">
-            <v>33.200000000000003</v>
-          </cell>
-          <cell r="B74">
-            <v>2724.0789999999993</v>
-          </cell>
-          <cell r="D74">
-            <v>44</v>
-          </cell>
-          <cell r="E74">
-            <v>2736.7600000000007</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="A75">
-            <v>33.5</v>
-          </cell>
-          <cell r="B75">
-            <v>2724.1639999999993</v>
-          </cell>
-          <cell r="D75">
-            <v>44.5</v>
-          </cell>
-          <cell r="E75">
-            <v>2736.9150000000009</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="A76">
-            <v>34</v>
-          </cell>
-          <cell r="B76">
-            <v>2724.1839999999993</v>
-          </cell>
-          <cell r="D76">
-            <v>44.8</v>
-          </cell>
-          <cell r="E76">
-            <v>2736.8200000000011</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="A77">
-            <v>34.5</v>
-          </cell>
-          <cell r="B77">
-            <v>2724.2139999999995</v>
-          </cell>
-          <cell r="D77">
-            <v>45.099999999999994</v>
-          </cell>
-          <cell r="E77">
-            <v>2737.045000000001</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="A78">
-            <v>35</v>
-          </cell>
-          <cell r="B78">
-            <v>2724.1939999999995</v>
-          </cell>
-          <cell r="D78">
-            <v>45.599999999999994</v>
-          </cell>
-          <cell r="E78">
-            <v>2736.9650000000006</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="A79">
-            <v>35.299999999999997</v>
-          </cell>
-          <cell r="B79">
-            <v>2724.2289999999994</v>
-          </cell>
-          <cell r="D79">
-            <v>46</v>
-          </cell>
-          <cell r="E79">
-            <v>2737.1400000000008</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="A80">
-            <v>35.400000000000006</v>
-          </cell>
-          <cell r="B80">
-            <v>2724.5539999999992</v>
-          </cell>
-          <cell r="D80">
-            <v>46.5</v>
-          </cell>
-          <cell r="E80">
-            <v>2737.1850000000009</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="A81">
-            <v>35.700000000000003</v>
-          </cell>
-          <cell r="B81">
-            <v>2724.6239999999993</v>
-          </cell>
-          <cell r="D81">
-            <v>47</v>
-          </cell>
-          <cell r="E81">
-            <v>2737.1800000000007</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="A82">
-            <v>36.200000000000003</v>
-          </cell>
-          <cell r="B82">
-            <v>2724.5539999999992</v>
-          </cell>
-          <cell r="D82">
-            <v>47.2</v>
-          </cell>
-          <cell r="E82">
-            <v>2737.1950000000006</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="A83">
-            <v>36.5</v>
-          </cell>
-          <cell r="B83">
-            <v>2724.5839999999994</v>
-          </cell>
-          <cell r="D83">
-            <v>47.5</v>
-          </cell>
-          <cell r="E83">
-            <v>2737.4150000000009</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="A84">
-            <v>36.900000000000006</v>
-          </cell>
-          <cell r="B84">
-            <v>2724.5539999999992</v>
-          </cell>
-          <cell r="D84">
-            <v>48</v>
-          </cell>
-          <cell r="E84">
-            <v>2737.3400000000006</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="A85">
-            <v>37.200000000000003</v>
-          </cell>
-          <cell r="B85">
-            <v>2724.5739999999996</v>
-          </cell>
-          <cell r="D85">
-            <v>48.2</v>
-          </cell>
-          <cell r="E85">
-            <v>2737.2500000000009</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="A86">
-            <v>37.5</v>
-          </cell>
-          <cell r="B86">
-            <v>2724.6039999999994</v>
-          </cell>
-          <cell r="D86">
-            <v>49</v>
-          </cell>
-          <cell r="E86">
-            <v>2737.4650000000006</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="A87">
-            <v>38</v>
-          </cell>
-          <cell r="B87">
-            <v>2724.6389999999992</v>
-          </cell>
-          <cell r="D87">
-            <v>49.5</v>
-          </cell>
-          <cell r="E87">
-            <v>2737.4600000000009</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="A88">
-            <v>38.5</v>
-          </cell>
-          <cell r="B88">
-            <v>2724.6589999999992</v>
-          </cell>
-          <cell r="D88">
-            <v>49.900000000000006</v>
-          </cell>
-          <cell r="E88">
-            <v>2737.6850000000009</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="A89">
-            <v>39</v>
-          </cell>
-          <cell r="B89">
-            <v>2724.6439999999993</v>
-          </cell>
-          <cell r="D89">
-            <v>50.3</v>
-          </cell>
-          <cell r="E89">
-            <v>2737.6150000000007</v>
-          </cell>
-        </row>
-        <row r="90">
-          <cell r="A90">
-            <v>39.5</v>
-          </cell>
-          <cell r="B90">
-            <v>2724.6589999999992</v>
-          </cell>
-          <cell r="D90">
-            <v>50.900000000000006</v>
-          </cell>
-          <cell r="E90">
-            <v>2737.7900000000009</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="A91">
-            <v>39.700000000000003</v>
-          </cell>
-          <cell r="B91">
-            <v>2724.7439999999992</v>
-          </cell>
-          <cell r="D91">
-            <v>51.5</v>
-          </cell>
-          <cell r="E91">
-            <v>2737.7600000000007</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="A92">
-            <v>40</v>
-          </cell>
-          <cell r="B92">
-            <v>2724.7489999999993</v>
-          </cell>
-          <cell r="D92">
-            <v>52</v>
-          </cell>
-          <cell r="E92">
-            <v>2737.7850000000008</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="A93">
-            <v>40.5</v>
-          </cell>
-          <cell r="B93">
-            <v>2724.7439999999992</v>
-          </cell>
-          <cell r="D93">
-            <v>52.599999999999994</v>
-          </cell>
-          <cell r="E93">
-            <v>2737.8000000000006</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="A94">
-            <v>41</v>
-          </cell>
-          <cell r="B94">
-            <v>2724.7139999999995</v>
-          </cell>
-          <cell r="D94">
-            <v>53.2</v>
-          </cell>
-          <cell r="E94">
-            <v>2738.2050000000008</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="A95">
-            <v>41.5</v>
-          </cell>
-          <cell r="B95">
-            <v>2724.7439999999992</v>
-          </cell>
-          <cell r="D95">
-            <v>53.7</v>
-          </cell>
-          <cell r="E95">
-            <v>2738.2100000000009</v>
-          </cell>
-        </row>
-        <row r="96">
-          <cell r="D96">
-            <v>54</v>
-          </cell>
-          <cell r="E96">
-            <v>2738.0800000000008</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="D97">
-            <v>54.5</v>
-          </cell>
-          <cell r="E97">
-            <v>2738.0850000000009</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4552,1422 +3386,1644 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39439EB6-EECA-4B3D-9A71-9F49E573C4F8}">
-  <dimension ref="A1:K101"/>
+  <dimension ref="A1:M101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.21875" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="2" max="3" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="7" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="1"/>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>2721.752</v>
       </c>
-      <c r="D3" s="2">
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1">
         <v>0</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="2">
         <v>2732.8400000000011</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>0.29999999999999716</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>2721.7419999999997</v>
       </c>
-      <c r="D4" s="2">
+      <c r="C4" s="1"/>
+      <c r="E4" s="1">
         <v>0.70000000000000284</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="2">
         <v>2733.0300000000007</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>1</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>2721.7559999999999</v>
       </c>
-      <c r="D5" s="2">
+      <c r="C5" s="1"/>
+      <c r="E5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="2">
         <v>2732.9900000000007</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>1</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>2721.7619999999997</v>
       </c>
-      <c r="D6" s="2">
+      <c r="C6" s="1"/>
+      <c r="E6" s="1">
         <v>2</v>
       </c>
-      <c r="E6" s="3">
+      <c r="F6" s="2">
         <v>2732.9450000000011</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>1.5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>2721.732</v>
       </c>
-      <c r="D7" s="2">
+      <c r="C7" s="1"/>
+      <c r="E7" s="1">
         <v>3</v>
       </c>
-      <c r="E7" s="3">
+      <c r="F7" s="2">
         <v>2733.0400000000009</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+      <c r="G7" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>2</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>2721.732</v>
       </c>
-      <c r="D8" s="2">
+      <c r="C8" s="1"/>
+      <c r="E8" s="1">
         <v>4</v>
       </c>
-      <c r="E8" s="3">
+      <c r="F8" s="2">
         <v>2733.0900000000011</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>2.5</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>2721.7619999999997</v>
       </c>
-      <c r="D9" s="2">
+      <c r="C9" s="1"/>
+      <c r="E9" s="1">
         <v>5</v>
       </c>
-      <c r="E9" s="3">
+      <c r="F9" s="2">
         <v>2733.1450000000009</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>3.1000000000000014</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>2721.7819999999997</v>
       </c>
-      <c r="D10" s="2">
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1">
         <v>6</v>
       </c>
-      <c r="E10" s="3">
+      <c r="F10" s="2">
         <v>2733.2100000000009</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
         <v>3.5</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>2721.8069999999998</v>
       </c>
-      <c r="D11" s="2">
+      <c r="C11" s="1"/>
+      <c r="E11" s="1">
         <v>7</v>
       </c>
-      <c r="E11" s="3">
+      <c r="F11" s="2">
         <v>2733.2400000000007</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
         <v>4.1000000000000014</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>2721.8819999999996</v>
       </c>
-      <c r="D12" s="2">
+      <c r="C12" s="1"/>
+      <c r="E12" s="1">
         <v>8</v>
       </c>
-      <c r="E12" s="3">
+      <c r="F12" s="2">
         <v>2733.295000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
         <v>4.5</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>2721.962</v>
       </c>
-      <c r="D13" s="2">
+      <c r="C13" s="1"/>
+      <c r="E13" s="1">
         <v>9</v>
       </c>
-      <c r="E13" s="3">
+      <c r="F13" s="2">
         <v>2733.3300000000008</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
         <v>5</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>2721.962</v>
       </c>
-      <c r="D14" s="2">
+      <c r="C14" s="1"/>
+      <c r="E14" s="1">
         <v>9.6000000000000014</v>
       </c>
-      <c r="E14" s="3">
+      <c r="F14" s="2">
         <v>2733.3450000000007</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
         <v>5.5</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>2722.0119999999997</v>
       </c>
-      <c r="D15" s="2">
+      <c r="C15" s="1"/>
+      <c r="E15" s="1">
         <v>9.7999999999999972</v>
       </c>
-      <c r="E15" s="3">
+      <c r="F15" s="2">
         <v>2733.5850000000009</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
         <v>6</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>2722.047</v>
       </c>
-      <c r="D16" s="2">
+      <c r="C16" s="1"/>
+      <c r="E16" s="1">
         <v>10</v>
       </c>
-      <c r="E16" s="3">
+      <c r="F16" s="2">
         <v>2733.5700000000011</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
         <v>6.5</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>2722.0619999999999</v>
       </c>
-      <c r="D17" s="2">
+      <c r="C17" s="1"/>
+      <c r="E17" s="1">
         <v>11</v>
       </c>
-      <c r="E17" s="3">
+      <c r="F17" s="2">
         <v>2733.5950000000007</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
         <v>7</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>2722.0969999999998</v>
       </c>
-      <c r="D18" s="2">
+      <c r="C18" s="1"/>
+      <c r="E18" s="1">
         <v>11.600000000000001</v>
       </c>
-      <c r="E18" s="3">
+      <c r="F18" s="2">
         <v>2733.565000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
         <v>7.5</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>2722.1519999999996</v>
       </c>
-      <c r="D19" s="2">
+      <c r="C19" s="1"/>
+      <c r="E19" s="1">
         <v>12</v>
       </c>
-      <c r="E19" s="3">
+      <c r="F19" s="2">
         <v>2733.7250000000008</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="2"/>
+      <c r="I19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H19" s="2">
+      <c r="J19" s="1">
         <v>8.7599999999999997E-2</v>
       </c>
-      <c r="I19" s="2">
-        <f>1000*9.81*0.6*H19</f>
+      <c r="K19" s="1">
+        <f>1000*9.81*0.6*J19</f>
         <v>515.61360000000002</v>
       </c>
-      <c r="K19" s="2">
-        <f>AVERAGE(H19:H20)</f>
+      <c r="M19" s="1">
+        <f>AVERAGE(J19:J20)</f>
         <v>9.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
         <v>8</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>2722.1319999999996</v>
       </c>
-      <c r="D20" s="2">
+      <c r="C20" s="1"/>
+      <c r="E20" s="1">
         <v>13.200000000000003</v>
       </c>
-      <c r="E20" s="3">
+      <c r="F20" s="2">
         <v>2733.6150000000007</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="2"/>
+      <c r="I20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H20" s="2">
+      <c r="J20" s="1">
         <v>0.1014</v>
       </c>
-      <c r="I20" s="2">
-        <f>1000*9.81*0.6*H20</f>
+      <c r="K20" s="1">
+        <f>1000*9.81*0.6*J20</f>
         <v>596.84040000000005</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
         <v>8.5</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>2722.1419999999998</v>
       </c>
-      <c r="D21" s="2">
+      <c r="C21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="1">
         <v>13.5</v>
       </c>
-      <c r="E21" s="3">
+      <c r="F21" s="2">
         <v>2733.7400000000007</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
         <v>9</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>2722.2169999999996</v>
       </c>
-      <c r="D22" s="2">
+      <c r="C22" s="1"/>
+      <c r="E22" s="1">
         <v>13.600000000000001</v>
       </c>
-      <c r="E22" s="3">
+      <c r="F22" s="2">
         <v>2733.880000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
         <v>9.5</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>2722.1819999999998</v>
       </c>
-      <c r="D23" s="2">
+      <c r="C23" s="1"/>
+      <c r="E23" s="1">
         <v>14</v>
       </c>
-      <c r="E23" s="3">
+      <c r="F23" s="2">
         <v>2733.8750000000009</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
         <v>10</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>2722.2169999999996</v>
       </c>
-      <c r="D24" s="2">
+      <c r="C24" s="1"/>
+      <c r="E24" s="1">
         <v>14.600000000000001</v>
       </c>
-      <c r="E24" s="3">
+      <c r="F24" s="2">
         <v>2733.8300000000008</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
         <v>10.700000000000003</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>2722.2919999999999</v>
       </c>
-      <c r="D25" s="2">
+      <c r="C25" s="1"/>
+      <c r="E25" s="1">
         <v>15.299999999999997</v>
       </c>
-      <c r="E25" s="3">
+      <c r="F25" s="2">
         <v>2733.7650000000008</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
         <v>11.5</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>2722.3419999999996</v>
       </c>
-      <c r="D26" s="2">
+      <c r="C26" s="1"/>
+      <c r="E26" s="1">
         <v>15.700000000000003</v>
       </c>
-      <c r="E26" s="3">
+      <c r="F26" s="2">
         <v>2733.8700000000008</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
         <v>11.799999999999997</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>2722.4319999999998</v>
       </c>
-      <c r="D27" s="2">
+      <c r="C27" s="1"/>
+      <c r="E27" s="1">
         <v>16</v>
       </c>
-      <c r="E27" s="3">
+      <c r="F27" s="2">
         <v>2734.0350000000008</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
         <v>12.5</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>2722.4919999999997</v>
       </c>
-      <c r="D28" s="2">
+      <c r="C28" s="1"/>
+      <c r="E28" s="1">
         <v>17</v>
       </c>
-      <c r="E28" s="3">
+      <c r="F28" s="2">
         <v>2734.0400000000009</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
+      <c r="G28" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
         <v>13</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>2722.4719999999998</v>
       </c>
-      <c r="D29" s="2">
+      <c r="C29" s="1"/>
+      <c r="E29" s="1">
         <v>17.600000000000001</v>
       </c>
-      <c r="E29" s="3">
+      <c r="F29" s="2">
         <v>2734.0350000000008</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
         <v>13.5</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>2722.4869999999996</v>
       </c>
-      <c r="D30" s="2">
+      <c r="C30" s="1"/>
+      <c r="E30" s="1">
         <v>18</v>
       </c>
-      <c r="E30" s="3">
+      <c r="F30" s="2">
         <v>2734.1800000000007</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
+      <c r="G30" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
         <v>14</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>2722.5719999999997</v>
       </c>
-      <c r="D31" s="2">
+      <c r="C31" s="1"/>
+      <c r="E31" s="1">
         <v>18.5</v>
       </c>
-      <c r="E31" s="3">
+      <c r="F31" s="2">
         <v>2734.1150000000007</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
         <v>14.5</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>2722.6169999999997</v>
       </c>
-      <c r="D32" s="2">
+      <c r="C32" s="1"/>
+      <c r="E32" s="1">
         <v>19</v>
       </c>
-      <c r="E32" s="3">
+      <c r="F32" s="2">
         <v>2734.1650000000009</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
         <v>15</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="1">
         <v>2722.587</v>
       </c>
-      <c r="D33" s="2">
+      <c r="C33" s="1"/>
+      <c r="E33" s="1">
         <v>20</v>
       </c>
-      <c r="E33" s="3">
+      <c r="F33" s="2">
         <v>2734.2850000000008</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
         <v>15.5</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="1">
         <v>2722.587</v>
       </c>
-      <c r="D34" s="2">
+      <c r="C34" s="1"/>
+      <c r="E34" s="1">
         <v>20.5</v>
       </c>
-      <c r="E34" s="3">
+      <c r="F34" s="2">
         <v>2734.3200000000006</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
         <v>16</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="1">
         <v>2722.5519999999997</v>
       </c>
-      <c r="D35" s="2">
+      <c r="C35" s="1"/>
+      <c r="E35" s="1">
         <v>21</v>
       </c>
-      <c r="E35" s="3">
+      <c r="F35" s="2">
         <v>2734.3450000000007</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
         <v>16.5</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="1">
         <v>2722.5789999999997</v>
       </c>
-      <c r="D36" s="2">
+      <c r="C36" s="1"/>
+      <c r="E36" s="1">
         <v>22</v>
       </c>
-      <c r="E36" s="3">
+      <c r="F36" s="2">
         <v>2734.380000000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="2">
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
         <v>17</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37" s="1">
         <v>2722.5619999999999</v>
       </c>
-      <c r="D37" s="2">
+      <c r="C37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="1">
         <v>23</v>
       </c>
-      <c r="E37" s="3">
+      <c r="F37" s="2">
         <v>2734.4300000000007</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="2">
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
         <v>17.5</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38" s="1">
         <v>2722.6519999999996</v>
       </c>
-      <c r="D38" s="2">
+      <c r="C38" s="1"/>
+      <c r="E38" s="1">
         <v>23.299999999999997</v>
       </c>
-      <c r="E38" s="3">
+      <c r="F38" s="2">
         <v>2734.3950000000009</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="2">
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
         <v>18.299999999999997</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39" s="1">
         <v>2722.6539999999995</v>
       </c>
-      <c r="D39" s="2">
+      <c r="C39" s="1"/>
+      <c r="E39" s="1">
         <v>23.6</v>
       </c>
-      <c r="E39" s="3">
+      <c r="F39" s="2">
         <v>2734.545000000001</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="2">
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
         <v>18.600000000000001</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40" s="1">
         <v>2722.7789999999995</v>
       </c>
-      <c r="D40" s="2">
+      <c r="C40" s="1"/>
+      <c r="E40" s="1">
         <v>24.6</v>
       </c>
-      <c r="E40" s="3">
+      <c r="F40" s="2">
         <v>2734.8450000000007</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="2">
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
         <v>19.100000000000001</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41" s="1">
         <v>2722.6989999999996</v>
       </c>
-      <c r="D41" s="2">
+      <c r="C41" s="1"/>
+      <c r="E41" s="1">
         <v>25</v>
       </c>
-      <c r="E41" s="3">
+      <c r="F41" s="2">
         <v>2734.5750000000007</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="2">
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
         <v>19.299999999999997</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="1">
         <v>2723.0039999999995</v>
       </c>
-      <c r="D42" s="2">
+      <c r="C42" s="1"/>
+      <c r="E42" s="1">
         <v>25.299999999999997</v>
       </c>
-      <c r="E42" s="3">
+      <c r="F42" s="2">
         <v>2734.5600000000009</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="2">
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
         <v>19.5</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="1">
         <v>2723.0239999999994</v>
       </c>
-      <c r="D43" s="2">
+      <c r="C43" s="1"/>
+      <c r="E43" s="1">
         <v>26</v>
       </c>
-      <c r="E43" s="3">
+      <c r="F43" s="2">
         <v>2735.0100000000007</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="2">
+      <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
         <v>20</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="1">
         <v>2723.0789999999997</v>
       </c>
-      <c r="D44" s="2">
+      <c r="C44" s="1"/>
+      <c r="E44" s="1">
         <v>26.700000000000003</v>
       </c>
-      <c r="E44" s="3">
+      <c r="F44" s="2">
         <v>2735.0800000000008</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="2">
+      <c r="G44" s="2"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
         <v>20.5</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="1">
         <v>2723.0739999999996</v>
       </c>
-      <c r="D45" s="2">
+      <c r="C45" s="1"/>
+      <c r="E45" s="1">
         <v>27</v>
       </c>
-      <c r="E45" s="3">
+      <c r="F45" s="2">
         <v>2735.025000000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="2">
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
         <v>20.700000000000003</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46" s="1">
         <v>2723.0039999999995</v>
       </c>
-      <c r="D46" s="2">
+      <c r="C46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="1">
         <v>27.1</v>
       </c>
-      <c r="E46" s="3">
+      <c r="F46" s="2">
         <v>2735.0000000000009</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="2">
+      <c r="G46" s="2"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
         <v>20.700000000000003</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="1">
         <v>2723.0989999999997</v>
       </c>
-      <c r="D47" s="2">
+      <c r="C47" s="1"/>
+      <c r="E47" s="1">
         <v>27.6</v>
       </c>
-      <c r="E47" s="3">
+      <c r="F47" s="2">
         <v>2735.2300000000009</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="2">
+      <c r="G47" s="2"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
         <v>21.4</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48" s="1">
         <v>2723.0489999999995</v>
       </c>
-      <c r="D48" s="2">
+      <c r="C48" s="1"/>
+      <c r="E48" s="1">
         <v>28</v>
       </c>
-      <c r="E48" s="3">
+      <c r="F48" s="2">
         <v>2735.1450000000009</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="2">
+      <c r="G48" s="2"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
         <v>21.6</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49" s="1">
         <v>2723.1789999999996</v>
       </c>
-      <c r="D49" s="2">
+      <c r="C49" s="1"/>
+      <c r="E49" s="1">
         <v>29</v>
       </c>
-      <c r="E49" s="3">
+      <c r="F49" s="2">
         <v>2735.1600000000008</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="2">
+      <c r="G49" s="2"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
         <v>22.715000000000003</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50" s="1">
         <v>2723.1889999999994</v>
       </c>
-      <c r="D50" s="2">
+      <c r="C50" s="1"/>
+      <c r="E50" s="1">
         <v>29.200000000000003</v>
       </c>
-      <c r="E50" s="3">
+      <c r="F50" s="2">
         <v>2735.3650000000007</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="2">
+      <c r="G50" s="2"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
         <v>23</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51" s="1">
         <v>2723.1889999999994</v>
       </c>
-      <c r="D51" s="2">
+      <c r="C51" s="1"/>
+      <c r="E51" s="1">
         <v>29.700000000000003</v>
       </c>
-      <c r="E51" s="3">
+      <c r="F51" s="2">
         <v>2735.2700000000009</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="2">
+      <c r="G51" s="2"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
         <v>23</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B52" s="1">
         <v>2723.1689999999994</v>
       </c>
-      <c r="D52" s="2">
+      <c r="C52" s="1"/>
+      <c r="E52" s="1">
         <v>30</v>
       </c>
-      <c r="E52" s="3">
+      <c r="F52" s="2">
         <v>2735.2150000000006</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="2">
+      <c r="G52" s="2"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
         <v>23.5</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53" s="1">
         <v>2723.1589999999997</v>
       </c>
-      <c r="D53" s="2">
+      <c r="C53" s="1"/>
+      <c r="E53" s="1">
         <v>30.5</v>
       </c>
-      <c r="E53" s="3">
+      <c r="F53" s="2">
         <v>2735.4600000000009</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="2">
+      <c r="G53" s="2"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
         <v>24</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54" s="1">
         <v>2723.1489999999994</v>
       </c>
-      <c r="D54" s="2">
+      <c r="C54" s="1"/>
+      <c r="E54" s="1">
         <v>31</v>
       </c>
-      <c r="E54" s="3">
+      <c r="F54" s="2">
         <v>2735.4150000000009</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="2">
+      <c r="G54" s="2"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
         <v>24.5</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B55" s="1">
         <v>2723.1589999999997</v>
       </c>
-      <c r="D55" s="2">
+      <c r="C55" s="1"/>
+      <c r="E55" s="1">
         <v>32</v>
       </c>
-      <c r="E55" s="3">
+      <c r="F55" s="2">
         <v>2735.4600000000009</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="2">
+      <c r="G55" s="2"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" s="1">
         <v>25</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B56" s="1">
         <v>2723.2389999999996</v>
       </c>
-      <c r="D56" s="2">
+      <c r="C56" s="1"/>
+      <c r="E56" s="1">
         <v>33</v>
       </c>
-      <c r="E56" s="3">
+      <c r="F56" s="2">
         <v>2735.4700000000007</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="2">
+      <c r="G56" s="2"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" s="1">
         <v>25.5</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B57" s="1">
         <v>2723.2589999999996</v>
       </c>
-      <c r="D57" s="2">
+      <c r="C57" s="1"/>
+      <c r="E57" s="1">
         <v>33.5</v>
       </c>
-      <c r="E57" s="3">
+      <c r="F57" s="2">
         <v>2735.4800000000009</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="2">
+      <c r="G57" s="2"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" s="1">
         <v>25.9</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58" s="1">
         <v>2723.5189999999993</v>
       </c>
-      <c r="D58" s="2">
+      <c r="C58" s="1"/>
+      <c r="E58" s="1">
         <v>34.5</v>
       </c>
-      <c r="E58" s="3">
+      <c r="F58" s="2">
         <v>2736.1250000000009</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="2">
+      <c r="G58" s="2"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" s="1">
         <v>26.5</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B59" s="1">
         <v>2723.4289999999996</v>
       </c>
-      <c r="D59" s="2">
+      <c r="C59" s="1"/>
+      <c r="E59" s="1">
         <v>35</v>
       </c>
-      <c r="E59" s="3">
+      <c r="F59" s="2">
         <v>2736.1150000000007</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" s="1">
         <v>26.9</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B60" s="1">
         <v>2723.4489999999996</v>
       </c>
-      <c r="D60" s="2">
+      <c r="C60" s="1"/>
+      <c r="E60" s="1">
         <v>36</v>
       </c>
-      <c r="E60" s="3">
+      <c r="F60" s="2">
         <v>2736.0900000000006</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="2">
+      <c r="G60" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" s="1">
         <v>26.9</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B61" s="1">
         <v>2723.4069999999997</v>
       </c>
-      <c r="D61" s="2">
+      <c r="C61" s="1"/>
+      <c r="E61" s="1">
         <v>36.299999999999997</v>
       </c>
-      <c r="E61" s="3">
+      <c r="F61" s="2">
         <v>2736.0350000000008</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="2">
+      <c r="G61" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" s="1">
         <v>27.5</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62" s="1">
         <v>2723.5189999999993</v>
       </c>
-      <c r="D62" s="2">
+      <c r="C62" s="1"/>
+      <c r="E62" s="1">
         <v>37</v>
       </c>
-      <c r="E62" s="3">
+      <c r="F62" s="2">
         <v>2736.420000000001</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" s="2">
+      <c r="G62" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" s="1">
         <v>27.799999999999997</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B63" s="1">
         <v>2723.6589999999997</v>
       </c>
-      <c r="D63" s="2">
+      <c r="C63" s="1"/>
+      <c r="E63" s="1">
         <v>37.599999999999994</v>
       </c>
-      <c r="E63" s="3">
+      <c r="F63" s="2">
         <v>2736.440000000001</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" s="2">
+      <c r="G63" s="2"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" s="1">
         <v>28</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B64" s="1">
         <v>2723.5789999999997</v>
       </c>
-      <c r="D64" s="2">
+      <c r="C64" s="1"/>
+      <c r="E64" s="1">
         <v>38</v>
       </c>
-      <c r="E64" s="3">
+      <c r="F64" s="2">
         <v>2736.4300000000007</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="2">
+      <c r="G64" s="2"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" s="1">
         <v>28.5</v>
       </c>
-      <c r="B65" s="2">
+      <c r="B65" s="1">
         <v>2723.7089999999994</v>
       </c>
-      <c r="D65" s="2">
+      <c r="C65" s="1"/>
+      <c r="E65" s="1">
         <v>39</v>
       </c>
-      <c r="E65" s="3">
+      <c r="F65" s="2">
         <v>2736.565000000001</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="2">
+      <c r="G65" s="2"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" s="1">
         <v>29</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B66" s="1">
         <v>2723.6689999999994</v>
       </c>
-      <c r="D66" s="2">
+      <c r="C66" s="1"/>
+      <c r="E66" s="1">
         <v>40</v>
       </c>
-      <c r="E66" s="3">
+      <c r="F66" s="2">
         <v>2736.5150000000008</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="2">
+      <c r="G66" s="2"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" s="1">
         <v>29.5</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B67" s="1">
         <v>2723.7089999999994</v>
       </c>
-      <c r="D67" s="2">
+      <c r="C67" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E67" s="1">
         <v>40.299999999999997</v>
       </c>
-      <c r="E67" s="3">
+      <c r="F67" s="2">
         <v>2736.7050000000008</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="2">
+      <c r="G67" s="2"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" s="1">
         <v>30</v>
       </c>
-      <c r="B68" s="2">
+      <c r="B68" s="1">
         <v>2723.8189999999995</v>
       </c>
-      <c r="D68" s="2">
+      <c r="C68" s="1"/>
+      <c r="E68" s="1">
         <v>41</v>
       </c>
-      <c r="E68" s="3">
+      <c r="F68" s="2">
         <v>2736.6450000000009</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" s="2">
+      <c r="G68" s="2"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69" s="1">
         <v>30.5</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B69" s="1">
         <v>2723.8389999999995</v>
       </c>
-      <c r="D69" s="2">
+      <c r="C69" s="1"/>
+      <c r="E69" s="1">
         <v>41.7</v>
       </c>
-      <c r="E69" s="3">
+      <c r="F69" s="2">
         <v>2736.610000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" s="2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70" s="1">
         <v>31</v>
       </c>
-      <c r="B70" s="2">
+      <c r="B70" s="1">
         <v>2723.8389999999995</v>
       </c>
-      <c r="D70" s="2">
+      <c r="C70" s="1"/>
+      <c r="E70" s="1">
         <v>42</v>
       </c>
-      <c r="E70" s="3">
+      <c r="F70" s="2">
         <v>2736.7650000000008</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71" s="1">
         <v>31.5</v>
       </c>
-      <c r="B71" s="2">
+      <c r="B71" s="1">
         <v>2723.8789999999995</v>
       </c>
-      <c r="D71" s="2">
+      <c r="C71" s="1"/>
+      <c r="E71" s="1">
         <v>42.599999999999994</v>
       </c>
-      <c r="E71" s="3">
+      <c r="F71" s="2">
         <v>2736.7890000000007</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" s="2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" s="1">
         <v>32</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B72" s="1">
         <v>2723.9239999999995</v>
       </c>
-      <c r="D72" s="2">
+      <c r="C72" s="1"/>
+      <c r="E72" s="1">
         <v>43</v>
       </c>
-      <c r="E72" s="3">
+      <c r="F72" s="2">
         <v>2736.8000000000011</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73" s="2">
+      <c r="G72" s="2"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73" s="1">
         <v>32.5</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B73" s="1">
         <v>2723.8839999999996</v>
       </c>
-      <c r="D73" s="2">
+      <c r="C73" s="1"/>
+      <c r="E73" s="1">
         <v>43.5</v>
       </c>
-      <c r="E73" s="3">
+      <c r="F73" s="2">
         <v>2736.735000000001</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74" s="2">
+      <c r="G73" s="2"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" s="1">
         <v>33.200000000000003</v>
       </c>
-      <c r="B74" s="2">
+      <c r="B74" s="1">
         <v>2724.0789999999993</v>
       </c>
-      <c r="D74" s="2">
+      <c r="C74" s="1"/>
+      <c r="E74" s="1">
         <v>44</v>
       </c>
-      <c r="E74" s="3">
+      <c r="F74" s="2">
         <v>2736.7600000000007</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" s="2">
+      <c r="G74" s="2"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" s="1">
         <v>33.5</v>
       </c>
-      <c r="B75" s="2">
+      <c r="B75" s="1">
         <v>2724.1639999999993</v>
       </c>
-      <c r="D75" s="2">
+      <c r="C75" s="1"/>
+      <c r="E75" s="1">
         <v>44.5</v>
       </c>
-      <c r="E75" s="3">
+      <c r="F75" s="2">
         <v>2736.9150000000009</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" s="2">
+      <c r="G75" s="2"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
         <v>34</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B76" s="1">
         <v>2724.1839999999993</v>
       </c>
-      <c r="D76" s="2">
+      <c r="C76" s="1"/>
+      <c r="E76" s="1">
         <v>44.8</v>
       </c>
-      <c r="E76" s="3">
+      <c r="F76" s="2">
         <v>2736.8200000000011</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77" s="2">
+      <c r="G76" s="2"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77" s="1">
         <v>34.5</v>
       </c>
-      <c r="B77" s="2">
+      <c r="B77" s="1">
         <v>2724.2139999999995</v>
       </c>
-      <c r="D77" s="2">
+      <c r="C77" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E77" s="1">
         <v>45.099999999999994</v>
       </c>
-      <c r="E77" s="3">
+      <c r="F77" s="2">
         <v>2737.045000000001</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A78" s="2">
+      <c r="G77" s="2"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A78" s="1">
         <v>35</v>
       </c>
-      <c r="B78" s="2">
+      <c r="B78" s="1">
         <v>2724.1939999999995</v>
       </c>
-      <c r="D78" s="2">
+      <c r="C78" s="1"/>
+      <c r="E78" s="1">
         <v>45.599999999999994</v>
       </c>
-      <c r="E78" s="3">
+      <c r="F78" s="2">
         <v>2736.9650000000006</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A79" s="2">
+      <c r="G78" s="2"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A79" s="1">
         <v>35.299999999999997</v>
       </c>
-      <c r="B79" s="2">
+      <c r="B79" s="1">
         <v>2724.2289999999994</v>
       </c>
-      <c r="D79" s="2">
+      <c r="C79" s="1"/>
+      <c r="E79" s="1">
         <v>46</v>
       </c>
-      <c r="E79" s="3">
+      <c r="F79" s="2">
         <v>2737.1400000000008</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A80" s="2">
+      <c r="G79" s="2"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A80" s="1">
         <v>35.400000000000006</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B80" s="1">
         <v>2724.5539999999992</v>
       </c>
-      <c r="D80" s="2">
+      <c r="C80" s="1"/>
+      <c r="E80" s="1">
         <v>46.5</v>
       </c>
-      <c r="E80" s="3">
+      <c r="F80" s="2">
         <v>2737.1850000000009</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A81" s="2">
+      <c r="G80" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81" s="1">
         <v>35.700000000000003</v>
       </c>
-      <c r="B81" s="2">
+      <c r="B81" s="1">
         <v>2724.6239999999993</v>
       </c>
-      <c r="D81" s="2">
+      <c r="C81" s="1"/>
+      <c r="E81" s="1">
         <v>47</v>
       </c>
-      <c r="E81" s="3">
+      <c r="F81" s="2">
         <v>2737.1800000000007</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A82" s="2">
+      <c r="G81" s="2"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
         <v>36.200000000000003</v>
       </c>
-      <c r="B82" s="2">
+      <c r="B82" s="1">
         <v>2724.5539999999992</v>
       </c>
-      <c r="D82" s="2">
+      <c r="C82" s="1"/>
+      <c r="E82" s="1">
         <v>47.2</v>
       </c>
-      <c r="E82" s="3">
+      <c r="F82" s="2">
         <v>2737.1950000000006</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A83" s="2">
+      <c r="G82" s="2"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A83" s="1">
         <v>36.5</v>
       </c>
-      <c r="B83" s="2">
+      <c r="B83" s="1">
         <v>2724.5839999999994</v>
       </c>
-      <c r="D83" s="2">
+      <c r="C83" s="1"/>
+      <c r="E83" s="1">
         <v>47.5</v>
       </c>
-      <c r="E83" s="3">
+      <c r="F83" s="2">
         <v>2737.4150000000009</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A84" s="2">
+      <c r="G83" s="2"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A84" s="1">
         <v>36.900000000000006</v>
       </c>
-      <c r="B84" s="2">
+      <c r="B84" s="1">
         <v>2724.5539999999992</v>
       </c>
-      <c r="D84" s="2">
+      <c r="C84" s="1"/>
+      <c r="E84" s="1">
         <v>48</v>
       </c>
-      <c r="E84" s="3">
+      <c r="F84" s="2">
         <v>2737.3400000000006</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A85" s="2">
+      <c r="G84" s="2"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A85" s="1">
         <v>37.200000000000003</v>
       </c>
-      <c r="B85" s="2">
+      <c r="B85" s="1">
         <v>2724.5739999999996</v>
       </c>
-      <c r="D85" s="2">
+      <c r="C85" s="1"/>
+      <c r="E85" s="1">
         <v>48.2</v>
       </c>
-      <c r="E85" s="3">
+      <c r="F85" s="2">
         <v>2737.2500000000009</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A86" s="2">
+      <c r="G85" s="2"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A86" s="1">
         <v>37.5</v>
       </c>
-      <c r="B86" s="2">
+      <c r="B86" s="1">
         <v>2724.6039999999994</v>
       </c>
-      <c r="D86" s="2">
+      <c r="C86" s="1"/>
+      <c r="E86" s="1">
         <v>49</v>
       </c>
-      <c r="E86" s="3">
+      <c r="F86" s="2">
         <v>2737.4650000000006</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A87" s="2">
+      <c r="G86" s="2"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A87" s="1">
         <v>38</v>
       </c>
-      <c r="B87" s="2">
+      <c r="B87" s="1">
         <v>2724.6389999999992</v>
       </c>
-      <c r="D87" s="2">
+      <c r="C87" s="1"/>
+      <c r="E87" s="1">
         <v>49.5</v>
       </c>
-      <c r="E87" s="3">
+      <c r="F87" s="2">
         <v>2737.4600000000009</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A88" s="2">
+      <c r="G87" s="2"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A88" s="1">
         <v>38.5</v>
       </c>
-      <c r="B88" s="2">
+      <c r="B88" s="1">
         <v>2724.6589999999992</v>
       </c>
-      <c r="D88" s="2">
+      <c r="C88" s="1"/>
+      <c r="E88" s="1">
         <v>49.900000000000006</v>
       </c>
-      <c r="E88" s="3">
+      <c r="F88" s="2">
         <v>2737.6850000000009</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A89" s="2">
+      <c r="G88" s="2"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A89" s="1">
         <v>39</v>
       </c>
-      <c r="B89" s="2">
+      <c r="B89" s="1">
         <v>2724.6439999999993</v>
       </c>
-      <c r="D89" s="2">
+      <c r="C89" s="1"/>
+      <c r="E89" s="1">
         <v>50.3</v>
       </c>
-      <c r="E89" s="3">
+      <c r="F89" s="2">
         <v>2737.6150000000007</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A90" s="2">
+      <c r="G89" s="2"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A90" s="1">
         <v>39.5</v>
       </c>
-      <c r="B90" s="2">
+      <c r="B90" s="1">
         <v>2724.6589999999992</v>
       </c>
-      <c r="D90" s="2">
+      <c r="C90" s="1"/>
+      <c r="E90" s="1">
         <v>50.900000000000006</v>
       </c>
-      <c r="E90" s="3">
+      <c r="F90" s="2">
         <v>2737.7900000000009</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A91" s="2">
+      <c r="G90" s="2"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A91" s="1">
         <v>39.700000000000003</v>
       </c>
-      <c r="B91" s="2">
+      <c r="B91" s="1">
         <v>2724.7439999999992</v>
       </c>
-      <c r="D91" s="2">
+      <c r="C91" s="1"/>
+      <c r="E91" s="1">
         <v>51.5</v>
       </c>
-      <c r="E91" s="3">
+      <c r="F91" s="2">
         <v>2737.7600000000007</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A92" s="2">
+      <c r="G91" s="2"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A92" s="1">
         <v>40</v>
       </c>
-      <c r="B92" s="2">
+      <c r="B92" s="1">
         <v>2724.7489999999993</v>
       </c>
-      <c r="D92" s="2">
+      <c r="C92" s="1"/>
+      <c r="E92" s="1">
         <v>52</v>
       </c>
-      <c r="E92" s="3">
+      <c r="F92" s="2">
         <v>2737.7850000000008</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A93" s="2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A93" s="1">
         <v>40.5</v>
       </c>
-      <c r="B93" s="2">
+      <c r="B93" s="1">
         <v>2724.7439999999992</v>
       </c>
-      <c r="D93" s="2">
+      <c r="C93" s="1"/>
+      <c r="E93" s="1">
         <v>52.599999999999994</v>
       </c>
-      <c r="E93" s="3">
+      <c r="F93" s="2">
         <v>2737.8000000000006</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A94" s="2">
+      <c r="G93" s="2"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A94" s="1">
         <v>41</v>
       </c>
-      <c r="B94" s="2">
+      <c r="B94" s="1">
         <v>2724.7139999999995</v>
       </c>
-      <c r="D94" s="2">
+      <c r="C94" s="1"/>
+      <c r="E94" s="1">
         <v>53.2</v>
       </c>
-      <c r="E94" s="3">
+      <c r="F94" s="2">
         <v>2738.2050000000008</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A95" s="2">
+      <c r="G94" s="2"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A95" s="1">
         <v>41.5</v>
       </c>
-      <c r="B95" s="2">
+      <c r="B95" s="1">
         <v>2724.7439999999992</v>
       </c>
-      <c r="D95" s="2">
+      <c r="C95" s="1"/>
+      <c r="E95" s="1">
         <v>53.7</v>
       </c>
-      <c r="E95" s="3">
+      <c r="F95" s="2">
         <v>2738.2100000000009</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D96" s="2">
+      <c r="G95" s="2"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E96" s="1">
         <v>54</v>
       </c>
-      <c r="E96" s="3">
+      <c r="F96" s="2">
         <v>2738.0800000000008</v>
       </c>
-    </row>
-    <row r="97" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D97" s="2">
+      <c r="G96" s="2"/>
+    </row>
+    <row r="97" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E97" s="1">
         <v>54.5</v>
       </c>
-      <c r="E97" s="3">
+      <c r="F97" s="2">
         <v>2738.0850000000009</v>
       </c>
-    </row>
-    <row r="98" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D98" s="2">
+      <c r="G97" s="2"/>
+    </row>
+    <row r="98" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E98" s="1">
         <v>55.099999999999994</v>
       </c>
-      <c r="E98" s="3">
+      <c r="F98" s="2">
         <v>2738.1100000000006</v>
       </c>
-    </row>
-    <row r="99" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D99" s="2">
+      <c r="G98" s="2"/>
+    </row>
+    <row r="99" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E99" s="1">
         <v>55.900000000000006</v>
       </c>
-      <c r="E99" s="3">
+      <c r="F99" s="2">
         <v>2738.4050000000007</v>
       </c>
-    </row>
-    <row r="100" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D100" s="2">
+      <c r="G99" s="2"/>
+    </row>
+    <row r="100" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E100" s="1">
         <v>56.5</v>
       </c>
-      <c r="E100" s="3">
+      <c r="F100" s="2">
         <v>2738.3650000000007</v>
       </c>
-    </row>
-    <row r="101" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D101" s="2">
+      <c r="G100" s="2"/>
+    </row>
+    <row r="101" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E101" s="1">
         <v>58</v>
       </c>
-      <c r="E101" s="3">
+      <c r="F101" s="2">
         <v>2738.190000000001</v>
       </c>
+      <c r="G101" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>